<commit_message>
added input data and examples for demeter
</commit_message>
<xml_diff>
--- a/2021_demeter/example_infoFile.xlsx
+++ b/2021_demeter/example_infoFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mspg/Documents/GitHub/semiautomaticrefinement/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mspg/Documents/GitHub/cobratoolbox/papers/2021_demeter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24DD4D2-F62A-3748-8D1C-0C46AA45AC99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AF4BDC-59B3-6346-B18B-8DA853BECDD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="460" windowWidth="24880" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="460" windowWidth="24880" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="77">
   <si>
     <t>Phylum</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Strain</t>
   </si>
   <si>
-    <t>Input_Model</t>
-  </si>
-  <si>
     <t>Acetitomaculum_ruminis_DSM_5522</t>
   </si>
   <si>
@@ -193,13 +190,85 @@
   </si>
   <si>
     <t>NCBI Taxonomy ID</t>
+  </si>
+  <si>
+    <t>PubSeedID</t>
+  </si>
+  <si>
+    <t>2 - complete comparative genomics; 1 - certain comparative genomics; 0 - no comparative genomics</t>
+  </si>
+  <si>
+    <t>MicrobeID</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Present in AGORA2</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Achromobacter_insuavis_AXX_A</t>
+  </si>
+  <si>
+    <t>Achromobacter xylosoxidans AXX-A (1003200.3)</t>
+  </si>
+  <si>
+    <t>Achromobacter xylosoxidans AXX-A</t>
+  </si>
+  <si>
+    <t>Achromobacter insuavis</t>
+  </si>
+  <si>
+    <t>Achromobacter</t>
+  </si>
+  <si>
+    <t>Alcaligenaceae</t>
+  </si>
+  <si>
+    <t>Burkholderiales</t>
+  </si>
+  <si>
+    <t>Betaproteobacteria</t>
+  </si>
+  <si>
+    <t>Acinetobacter_pittii_TG6411</t>
+  </si>
+  <si>
+    <t>Acinetobacter pittii TG6411 (1221309.3)</t>
+  </si>
+  <si>
+    <t>Acinetobacter pittii TG6411</t>
+  </si>
+  <si>
+    <t>Acinetobacter pittii</t>
+  </si>
+  <si>
+    <t>Acinetobacter</t>
+  </si>
+  <si>
+    <t>Moraxellaceae</t>
+  </si>
+  <si>
+    <t>Pseudomonadales</t>
+  </si>
+  <si>
+    <t>Gammaproteobacteria</t>
+  </si>
+  <si>
+    <t>Annotation version ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,6 +290,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -244,11 +326,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text 3" xfId="1" xr:uid="{60C46832-D80F-0244-8E52-7350A1B65906}"/>
@@ -530,251 +614,412 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.33203125" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.5" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
-    <col min="8" max="9" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="38.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="31.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="10" max="11" width="15.6640625" customWidth="1"/>
+    <col min="12" max="12" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <v>1003200</v>
+      </c>
+      <c r="L2">
+        <v>1003200.3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>1221309</v>
+      </c>
+      <c r="L3">
+        <v>1221309.3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="B4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="5">
         <v>0</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4">
+        <v>1120918</v>
+      </c>
+      <c r="M4" t="s">
         <v>50</v>
       </c>
+      <c r="N4" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5">
+        <v>1118154</v>
+      </c>
+      <c r="M5" t="s">
+        <v>50</v>
+      </c>
+      <c r="N5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
         <v>26</v>
       </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="J6" t="s">
         <v>6</v>
       </c>
-      <c r="I2">
-        <v>1120918</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="K6">
+        <v>1350467</v>
+      </c>
+      <c r="M6" t="s">
+        <v>50</v>
+      </c>
+      <c r="N6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7">
+        <v>1401068</v>
+      </c>
+      <c r="M7" t="s">
         <v>51</v>
       </c>
+      <c r="N7" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>1410669</v>
+      </c>
+      <c r="M8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" t="s">
         <v>6</v>
       </c>
-      <c r="I3">
-        <v>1118154</v>
-      </c>
-      <c r="J3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4">
-        <v>1350467</v>
-      </c>
-      <c r="J4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5">
-        <v>1401068</v>
-      </c>
-      <c r="J5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>1410669</v>
-      </c>
-      <c r="J6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7">
+      <c r="K9">
         <v>699248</v>
       </c>
-      <c r="J7" t="s">
-        <v>51</v>
+      <c r="M9" t="s">
+        <v>50</v>
+      </c>
+      <c r="N9" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H6">
-    <sortCondition ref="A2:A6"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J8">
+    <sortCondition ref="A4:A8"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
further changes to DEMETER
</commit_message>
<xml_diff>
--- a/2021_demeter/example_infoFile.xlsx
+++ b/2021_demeter/example_infoFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mspg/Documents/GitHub/cobratoolbox/papers/2021_demeter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AF4BDC-59B3-6346-B18B-8DA853BECDD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEC22F8-DD8B-9D45-A92D-DC1BD65D119B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="460" windowWidth="24880" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2600" yWindow="460" windowWidth="24880" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="93">
   <si>
     <t>Phylum</t>
   </si>
@@ -262,6 +262,54 @@
   </si>
   <si>
     <t>Annotation version ID</t>
+  </si>
+  <si>
+    <t>Clostridioides_difficile_630</t>
+  </si>
+  <si>
+    <t>Clostridium difficile 630 (272563.8)</t>
+  </si>
+  <si>
+    <t>Clostridioides difficile 630</t>
+  </si>
+  <si>
+    <t>Clostridioides difficile</t>
+  </si>
+  <si>
+    <t>Clostridioides</t>
+  </si>
+  <si>
+    <t>Peptostreptococcaceae</t>
+  </si>
+  <si>
+    <t>Clostridiales</t>
+  </si>
+  <si>
+    <t>Clostridia</t>
+  </si>
+  <si>
+    <t>Lactobacillus_jensenii_269_3</t>
+  </si>
+  <si>
+    <t>Lactobacillus jensenii 269-3 (596325.3)</t>
+  </si>
+  <si>
+    <t>Lactobacillus jensenii 269-3</t>
+  </si>
+  <si>
+    <t>Lactobacillus jensenii</t>
+  </si>
+  <si>
+    <t>Lactobacillus</t>
+  </si>
+  <si>
+    <t>Lactobacillaceae</t>
+  </si>
+  <si>
+    <t>Lactobacillales</t>
+  </si>
+  <si>
+    <t>Bacilli</t>
   </si>
 </sst>
 </file>
@@ -614,20 +662,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.33203125" customWidth="1"/>
     <col min="2" max="2" width="38.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="31.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="22.5" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
     <col min="7" max="7" width="21.1640625" customWidth="1"/>
@@ -773,89 +822,95 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="C4" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="J4" t="s">
         <v>6</v>
       </c>
       <c r="K4">
-        <v>1120918</v>
+        <v>272563</v>
+      </c>
+      <c r="L4">
+        <v>272563.8</v>
       </c>
       <c r="M4" t="s">
         <v>50</v>
       </c>
       <c r="N4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="C5" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="J5" t="s">
         <v>6</v>
       </c>
       <c r="K5">
-        <v>1118154</v>
+        <v>596325</v>
+      </c>
+      <c r="L5">
+        <v>596325.30000000005</v>
       </c>
       <c r="M5" t="s">
         <v>50</v>
       </c>
       <c r="N5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>56</v>
@@ -864,28 +919,28 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J6" t="s">
         <v>6</v>
       </c>
       <c r="K6">
-        <v>1350467</v>
+        <v>1120918</v>
       </c>
       <c r="M6" t="s">
         <v>50</v>
@@ -896,7 +951,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>56</v>
@@ -905,31 +960,31 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="H7" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="J7" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="K7">
-        <v>1401068</v>
+        <v>1118154</v>
       </c>
       <c r="M7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N7" t="s">
         <v>59</v>
@@ -937,7 +992,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>56</v>
@@ -946,31 +1001,31 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="H8" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="I8" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="J8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K8">
-        <v>1410669</v>
+        <v>1350467</v>
       </c>
       <c r="M8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N8" t="s">
         <v>59</v>
@@ -978,7 +1033,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>56</v>
@@ -987,39 +1042,121 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H9" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="I9" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="J9" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="K9">
-        <v>699248</v>
+        <v>1401068</v>
       </c>
       <c r="M9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N9" t="s">
         <v>59</v>
       </c>
     </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>1410669</v>
+      </c>
+      <c r="M10" t="s">
+        <v>51</v>
+      </c>
+      <c r="N10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>699248</v>
+      </c>
+      <c r="M11" t="s">
+        <v>50</v>
+      </c>
+      <c r="N11" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J8">
-    <sortCondition ref="A4:A8"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:J10">
+    <sortCondition ref="A6:A10"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>